<commit_message>
config input as dynamically
change the config file to take the locations in dynamically
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8940"/>
+    <workbookView windowWidth="28800" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
     <t>input_File</t>
   </si>
   <si>
-    <t>C:\Users\PasinduPe\Documents\UiPath\RPAChallengeProject\Data\Input\Challenge.xlsx</t>
+    <t>Data\Input\Challenge.xlsx</t>
   </si>
   <si>
     <t>input file Location</t>
@@ -94,7 +94,7 @@
     <t>ScreenShotsPath</t>
   </si>
   <si>
-    <t>C:\Users\PasinduPe\Documents\UiPath\RPAChallengeProject\ScreenShot\</t>
+    <t>ScreenShot\</t>
   </si>
   <si>
     <t>Non Error Screen Shots Saved in this path</t>
@@ -103,7 +103,7 @@
     <t>ErrorScreenShotsPath</t>
   </si>
   <si>
-    <t>C:\Users\PasinduPe\Documents\UiPath\RPAChallengeProject\ErrorScreenShot\</t>
+    <t>ErrorScreenShot\</t>
   </si>
   <si>
     <t>Error Screen Shots Saved in this path</t>
@@ -112,7 +112,7 @@
     <t>Output_Location</t>
   </si>
   <si>
-    <t>C:\Users\PasinduPe\Documents\UiPath\RPAChallengeProject\Data\Output\</t>
+    <t>Data\Output\</t>
   </si>
   <si>
     <t>this location saved the final SS and the Output Text file</t>
@@ -1171,8 +1171,8 @@
   <sheetPr/>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4380952380952" defaultRowHeight="15" customHeight="1"/>

</xml_diff>